<commit_message>
Update Leave Card 3/20/2023 4:48 PM
</commit_message>
<xml_diff>
--- a/DONE 2-2-2023/DE LEON, ANALITA BAYOT.xlsx
+++ b/DONE 2-2-2023/DE LEON, ANALITA BAYOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\DONE 2-2-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02A666A-4F0C-4FDC-BA82-68FB43E76998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D810D657-0EF9-4B71-A704-F413B0C1B1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>PERIOD</t>
   </si>
@@ -206,6 +206,9 @@
   </si>
   <si>
     <t>DE LEON, ANALITA BAYOT</t>
+  </si>
+  <si>
+    <t>TOTAL LEAVE</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,15 +590,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -608,17 +602,29 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3254,7 +3260,7 @@
   </sheetPr>
   <dimension ref="A2:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="5532" topLeftCell="A76"/>
       <selection activeCell="B2" sqref="B2:C2"/>
       <selection pane="bottomLeft" activeCell="C76" sqref="C76:C77"/>
@@ -3287,14 +3293,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -3305,16 +3311,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56">
+      <c r="F3" s="53">
         <v>43101</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -3327,14 +3333,14 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -3360,18 +3366,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -5787,17 +5793,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -5866,14 +5872,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="55"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -5887,17 +5893,17 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="56">
+      <c r="F3" s="53">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F3:G3),"---------",'2018 LEAVE CREDITS'!F3:G3)</f>
         <v>43101</v>
       </c>
-      <c r="G3" s="50"/>
+      <c r="G3" s="54"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -5911,17 +5917,17 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="50" t="str">
+      <c r="F4" s="54" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="50"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="51"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -5947,18 +5953,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52" t="s">
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -8005,8 +8011,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8096,6 +8102,9 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -8117,6 +8126,10 @@
       <c r="L6" s="60"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="61">
+        <f>SUM('2018 LEAVE CREDITS'!$E$9,'2018 LEAVE CREDITS'!$I$9)</f>
+        <v>118</v>
+      </c>
       <c r="C7" s="37">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update Leave Card 4/11/2023 10:05 PM
</commit_message>
<xml_diff>
--- a/DONE 2-2-2023/DE LEON, ANALITA BAYOT.xlsx
+++ b/DONE 2-2-2023/DE LEON, ANALITA BAYOT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVECARD\DONE 2-2-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\LEAVE-CARD\DONE 2-2-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D810D657-0EF9-4B71-A704-F413B0C1B1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB127671-9CEF-40C7-94CB-D52322F86E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -587,8 +587,20 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -602,29 +614,17 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3260,10 +3260,10 @@
   </sheetPr>
   <dimension ref="A2:K134"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="5532" topLeftCell="A76"/>
-      <selection activeCell="B2" sqref="B2:C2"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76:C77"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2604" topLeftCell="A38" activePane="bottomLeft"/>
+      <selection activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft" activeCell="G64" sqref="G63:G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3285,62 +3285,62 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="56"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="57">
         <v>43101</v>
       </c>
-      <c r="G3" s="54"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -3366,18 +3366,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -3424,7 +3424,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])</f>
-        <v>52.5</v>
+        <v>53.75</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3434,7 +3434,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])</f>
-        <v>65.5</v>
+        <v>66.75</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -4834,13 +4834,15 @@
         <v>44986</v>
       </c>
       <c r="B78" s="20"/>
-      <c r="C78" s="13"/>
+      <c r="C78" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D78" s="39"/>
       <c r="E78" s="9"/>
       <c r="F78" s="20"/>
-      <c r="G78" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G78" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H78" s="39"/>
       <c r="I78" s="9"/>
@@ -5793,17 +5795,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -5838,10 +5840,10 @@
   </sheetPr>
   <dimension ref="A2:K130"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="5532" topLeftCell="A7" activePane="bottomLeft"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <pane ySplit="3516" activePane="bottomLeft"/>
       <selection activeCell="B4" sqref="B4:C4"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5863,71 +5865,71 @@
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="49" t="str">
+      <c r="B2" s="50" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B2:C2),"---------",'2018 LEAVE CREDITS'!B2:C2)</f>
         <v>DE LEON, ANALITA BAYOT</v>
       </c>
-      <c r="C2" s="49"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="56"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="50" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B3:C3),"",'2018 LEAVE CREDITS'!B3:C3)</f>
         <v/>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="57">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F3:G3),"---------",'2018 LEAVE CREDITS'!F3:G3)</f>
         <v>43101</v>
       </c>
-      <c r="G3" s="54"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="49" t="str">
+      <c r="B4" s="50" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!B4:C4),"---------",'2018 LEAVE CREDITS'!B4:C4)</f>
         <v>CASUAL</v>
       </c>
-      <c r="C4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="54" t="str">
+      <c r="F4" s="51" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="54"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="57"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
@@ -5953,18 +5955,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -8011,7 +8013,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -8030,17 +8032,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="J1" s="60" t="s">
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="J1" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -8118,17 +8120,17 @@
         <v>30</v>
       </c>
       <c r="G6" s="44"/>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="61">
+      <c r="A7" s="49">
         <f>SUM('2018 LEAVE CREDITS'!$E$9,'2018 LEAVE CREDITS'!$I$9)</f>
-        <v>118</v>
+        <v>120.5</v>
       </c>
       <c r="C7" s="37">
         <v>1</v>

</xml_diff>